<commit_message>
Update with one column
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20055" windowHeight="7695"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20055" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="check" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>nagpur</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -394,7 +397,7 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +407,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -415,8 +421,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>123</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -426,8 +435,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3">
+        <v>456</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -436,6 +448,9 @@
       </c>
       <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -459,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>